<commit_message>
Refactor: Hoja de Ruta Motorizados se ordena por fecha de creación, independiente al pedido
</commit_message>
<xml_diff>
--- a/public/formatos/formatoMotorizados_hoja_de_rutas.xlsx
+++ b/public/formatos/formatoMotorizados_hoja_de_rutas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\programador grobdi\Desktop\PROYECTOS_K_28\SISTEMA GROBDI\pedidos-grobdi\public\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D3AC7B-0CD6-473D-AAAC-22A999D504A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482CADBF-77A3-42A8-B122-89A900958D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E66DB4E7-AA44-4905-B79C-939A99177439}"/>
   </bookViews>
@@ -324,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -372,17 +372,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -407,14 +396,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1639,8 +1638,8 @@
   </sheetPr>
   <dimension ref="B1:R34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1688,14 +1687,14 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
       <c r="L2" s="5"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -1709,12 +1708,12 @@
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
       <c r="L3" s="8"/>
       <c r="M3"/>
       <c r="N3"/>
@@ -1728,14 +1727,14 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="33"/>
+      <c r="I4" s="28"/>
       <c r="J4" s="12" t="s">
         <v>3</v>
       </c>
@@ -1895,10 +1894,10 @@
       <c r="E12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="35"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="18" t="s">
         <v>14</v>
       </c>
@@ -1911,351 +1910,351 @@
       <c r="K12" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="28" t="s">
+      <c r="L12" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28" t="s">
+      <c r="M12" s="23"/>
+      <c r="N12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
       <c r="Q12" s="17"/>
       <c r="R12" s="17"/>
     </row>
     <row r="13" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13"/>
-      <c r="C13" s="23">
+      <c r="C13" s="31">
         <v>0</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="38"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
       <c r="Q13"/>
       <c r="R13"/>
     </row>
     <row r="14" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14"/>
-      <c r="C14" s="23">
+      <c r="C14" s="31">
         <v>1</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="38"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
       <c r="Q14"/>
       <c r="R14"/>
     </row>
     <row r="15" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15"/>
-      <c r="C15" s="23">
+      <c r="C15" s="31">
         <v>2</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="38"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
       <c r="Q15"/>
       <c r="R15"/>
     </row>
     <row r="16" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16"/>
-      <c r="C16" s="23">
+      <c r="C16" s="31">
         <v>3</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
       <c r="Q16"/>
       <c r="R16"/>
     </row>
     <row r="17" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17"/>
-      <c r="C17" s="23">
+      <c r="C17" s="31">
         <v>4</v>
       </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
       <c r="Q17"/>
       <c r="R17"/>
     </row>
     <row r="18" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18"/>
-      <c r="C18" s="23">
+      <c r="C18" s="31">
         <v>5</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="38"/>
-      <c r="O18" s="38"/>
-      <c r="P18" s="38"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
       <c r="Q18"/>
       <c r="R18"/>
     </row>
     <row r="19" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19"/>
-      <c r="C19" s="23">
+      <c r="C19" s="31">
         <v>6</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
       <c r="Q19"/>
       <c r="R19"/>
     </row>
     <row r="20" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20"/>
-      <c r="C20" s="23">
+      <c r="C20" s="31">
         <v>7</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
       <c r="Q20"/>
       <c r="R20"/>
     </row>
     <row r="21" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21"/>
-      <c r="C21" s="23">
+      <c r="C21" s="31">
         <v>8</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="38"/>
-      <c r="O21" s="38"/>
-      <c r="P21" s="38"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
       <c r="Q21"/>
       <c r="R21"/>
     </row>
     <row r="22" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22"/>
-      <c r="C22" s="23">
+      <c r="C22" s="31">
         <v>9</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="38"/>
-      <c r="O22" s="38"/>
-      <c r="P22" s="38"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
       <c r="Q22"/>
       <c r="R22"/>
     </row>
     <row r="23" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23"/>
-      <c r="C23" s="23">
+      <c r="C23" s="31">
         <v>10</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="38"/>
-      <c r="O23" s="38"/>
-      <c r="P23" s="38"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
       <c r="Q23"/>
       <c r="R23"/>
     </row>
     <row r="24" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24"/>
-      <c r="C24" s="23">
+      <c r="C24" s="31">
         <v>11</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="38"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
       <c r="Q24"/>
       <c r="R24"/>
     </row>
     <row r="25" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25"/>
-      <c r="C25" s="23">
+      <c r="C25" s="31">
         <v>12</v>
       </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
       <c r="Q25"/>
       <c r="R25"/>
     </row>
     <row r="26" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26"/>
-      <c r="C26" s="23">
+      <c r="C26" s="31">
         <v>13</v>
       </c>
-      <c r="D26" s="24"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="38"/>
-      <c r="P26" s="38"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
       <c r="Q26"/>
       <c r="R26"/>
     </row>
     <row r="27" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27"/>
-      <c r="C27" s="23">
+      <c r="C27" s="31">
         <v>14</v>
       </c>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="38"/>
-      <c r="O27" s="38"/>
-      <c r="P27" s="38"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="36"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="36"/>
       <c r="Q27"/>
       <c r="R27"/>
     </row>
     <row r="28" spans="2:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28"/>
-      <c r="C28" s="23">
+      <c r="C28" s="31">
         <v>15</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="38"/>
-      <c r="O28" s="38"/>
-      <c r="P28" s="38"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="36"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="36"/>
       <c r="Q28"/>
       <c r="R28"/>
     </row>
@@ -2375,60 +2374,60 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="F2:K3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:P26"/>
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="L27:M27"/>
     <mergeCell ref="N27:P27"/>
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="L28:M28"/>
     <mergeCell ref="N28:P28"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="F2:K3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="L12:M12"/>
   </mergeCells>
   <pageMargins left="0.36" right="0.52" top="0.45" bottom="0.19" header="0.23" footer="0.12"/>
   <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>

</xml_diff>